<commit_message>
add antibodies_path to IMC and regen
</commit_message>
<xml_diff>
--- a/docs/imc/imc-metadata.xlsx
+++ b/docs/imc/imc-metadata.xlsx
@@ -532,11 +532,24 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>Relative path to file with antibody information for this dataset.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AN1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>Relative path to file with ORCID IDs for contributors for this dataset.</t>
         </r>
       </text>
     </comment>
-    <comment ref="AN1" authorId="0">
+    <comment ref="AO1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -554,7 +567,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>donor_id</t>
   </si>
@@ -704,6 +717,9 @@
   </si>
   <si>
     <t>data_precision_bytes</t>
+  </si>
+  <si>
+    <t>antibodies_path</t>
   </si>
   <si>
     <t>contributors_path</t>
@@ -1058,7 +1074,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AN1"/>
+  <dimension ref="A1:AO1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1067,7 +1083,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:40">
+    <row r="1" spans="1:41">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1187,6 +1203,9 @@
       </c>
       <c r="AN1" s="1" t="s">
         <v>51</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add version + description: regen
</commit_message>
<xml_diff>
--- a/docs/imc/imc-metadata.xlsx
+++ b/docs/imc/imc-metadata.xlsx
@@ -38,11 +38,37 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>version</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>description</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>HuBMAP Display ID of the donor of the assayed tissue.</t>
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0">
+    <comment ref="D1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -55,7 +81,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="E1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -68,7 +94,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -81,7 +107,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -94,7 +120,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -107,7 +133,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -120,7 +146,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0">
+    <comment ref="J1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -133,7 +159,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -146,7 +172,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -159,7 +185,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0">
+    <comment ref="M1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -172,7 +198,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0">
+    <comment ref="N1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -185,7 +211,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0">
+    <comment ref="O1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -198,7 +224,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0">
+    <comment ref="P1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -211,7 +237,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0">
+    <comment ref="Q1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -224,7 +250,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0">
+    <comment ref="R1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -237,7 +263,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0">
+    <comment ref="S1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -250,7 +276,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0">
+    <comment ref="T1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -263,7 +289,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0">
+    <comment ref="U1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -276,7 +302,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0">
+    <comment ref="V1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -289,7 +315,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0">
+    <comment ref="W1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -302,7 +328,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="0">
+    <comment ref="X1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -315,7 +341,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="0">
+    <comment ref="Y1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -328,7 +354,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="0">
+    <comment ref="Z1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -341,7 +367,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y1" authorId="0">
+    <comment ref="AA1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -354,7 +380,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z1" authorId="0">
+    <comment ref="AB1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -367,7 +393,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA1" authorId="0">
+    <comment ref="AC1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -380,7 +406,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB1" authorId="0">
+    <comment ref="AD1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -393,7 +419,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC1" authorId="0">
+    <comment ref="AE1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -406,7 +432,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD1" authorId="0">
+    <comment ref="AF1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -419,7 +445,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AE1" authorId="0">
+    <comment ref="AG1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -432,7 +458,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF1" authorId="0">
+    <comment ref="AH1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -445,7 +471,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AG1" authorId="0">
+    <comment ref="AI1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -458,7 +484,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AH1" authorId="0">
+    <comment ref="AJ1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -471,7 +497,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI1" authorId="0">
+    <comment ref="AK1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -484,7 +510,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AJ1" authorId="0">
+    <comment ref="AL1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -497,7 +523,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK1" authorId="0">
+    <comment ref="AM1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -510,7 +536,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AL1" authorId="0">
+    <comment ref="AN1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -523,7 +549,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AM1" authorId="0">
+    <comment ref="AO1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -536,7 +562,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AN1" authorId="0">
+    <comment ref="AP1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -549,7 +575,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AO1" authorId="0">
+    <comment ref="AQ1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -567,7 +593,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
   <si>
     <t>donor_id</t>
   </si>
@@ -1074,7 +1106,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AO1"/>
+  <dimension ref="A1:AQ1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1083,7 +1115,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:41">
+    <row r="1" spans="1:43">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1112,16 +1144,16 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>16</v>
@@ -1148,10 +1180,10 @@
         <v>23</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>28</v>
@@ -1160,10 +1192,10 @@
         <v>29</v>
       </c>
       <c r="Z1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>33</v>
@@ -1190,13 +1222,13 @@
         <v>40</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="AM1" s="1" t="s">
         <v>50</v>
@@ -1207,49 +1239,51 @@
       <c r="AO1" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="AP1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="20">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: mass_spectrometry_imaging." sqref="I2:I1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: mass_spectrometry_imaging." sqref="K2:K1048576">
       <formula1>'assay_category list'!$A$1:$A$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: Imaging Mass Cytometry." sqref="J2:J1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: Imaging Mass Cytometry." sqref="L2:L1048576">
       <formula1>'assay_type list'!$A$1:$A$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: protein." sqref="K2:K1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: protein." sqref="M2:M1048576">
       <formula1>'analyte_class list'!$A$1:$A$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a boolean" error="The values in this column must be &quot;TRUE&quot; or &quot;FALSE&quot;." sqref="L2:L1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a boolean" error="The values in this column must be &quot;TRUE&quot; or &quot;FALSE&quot;." sqref="N2:N1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not an integer" error="The values in this column must be integers." sqref="S2:S1048576">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not an integer" error="The values in this column must be integers." sqref="U2:U1048576">
       <formula1>-2147483647</formula1>
       <formula2>2147483647</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="T2:T1048576">
-      <formula1>-1e+307</formula1>
-      <formula2>1e+307</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: um / nm." sqref="U2:U1048576">
-      <formula1>'ablation_dista...s_x_units list'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="V2:V1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: um / nm." sqref="W2:W1048576">
-      <formula1>'ablation_dista...s_y_units list'!$A$1:$A$2</formula1>
+      <formula1>'ablation_dista...s_x_units list'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="X2:X1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: Hz." sqref="Y2:Y1048576">
-      <formula1>'ablation_frequency_unit list'!$A$1:$A$1</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AA2:AA1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: um / nm." sqref="Y2:Y1048576">
+      <formula1>'ablation_dista...s_y_units list'!$A$1:$A$2</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="Z2:Z1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: Hz." sqref="AA2:AA1048576">
+      <formula1>'ablation_frequency_unit list'!$A$1:$A$1</formula1>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AC2:AC1048576">
       <formula1>-1e+307</formula1>
@@ -1259,23 +1293,27 @@
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: um." sqref="AF2:AF1048576">
-      <formula1>'max_x_width_unit list'!$A$1:$A$1</formula1>
-    </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AG2:AG1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: um." sqref="AH2:AH1048576">
+      <formula1>'max_x_width_unit list'!$A$1:$A$1</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AI2:AI1048576">
+      <formula1>-1e+307</formula1>
+      <formula2>1e+307</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: um." sqref="AJ2:AJ1048576">
       <formula1>'max_y_height_unit list'!$A$1:$A$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: float / integer / string." sqref="AI2:AI1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: float / integer / string." sqref="AK2:AK1048576">
       <formula1>'segment_data_format list'!$A$1:$A$3</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: dual count / pulse count / intensity value." sqref="AJ2:AJ1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: dual count / pulse count / intensity value." sqref="AL2:AL1048576">
       <formula1>'signal_type list'!$A$1:$A$3</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AL2:AL1048576">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AN2:AN1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
@@ -1295,17 +1333,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1323,17 +1361,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1351,7 +1389,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1369,7 +1407,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1387,7 +1425,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1405,12 +1443,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1428,12 +1466,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1451,7 +1489,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1469,7 +1507,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1487,7 +1525,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>